<commit_message>
mocks - home page
</commit_message>
<xml_diff>
--- a/notes/bmhs_details.xlsx
+++ b/notes/bmhs_details.xlsx
@@ -4,28 +4,108 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="pages" sheetId="1" r:id="rId1"/>
     <sheet name="database" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="keywords" sheetId="3" r:id="rId3"/>
+    <sheet name="imp links" sheetId="4" r:id="rId4"/>
+    <sheet name="Ref web sites" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>home page</t>
+  </si>
+  <si>
+    <t>Checkout page</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Register</t>
+  </si>
+  <si>
+    <t>Email verification</t>
+  </si>
+  <si>
+    <t>Booking Confirmation</t>
+  </si>
+  <si>
+    <t>Facebook connect</t>
+  </si>
+  <si>
+    <t>user dashboard</t>
+  </si>
+  <si>
+    <t>Profile</t>
+  </si>
+  <si>
+    <t>Change password</t>
+  </si>
+  <si>
+    <t>Read/write reviews</t>
+  </si>
+  <si>
+    <t>See transactions</t>
+  </si>
+  <si>
+    <t>listing page</t>
+  </si>
+  <si>
+    <t>Grid view</t>
+  </si>
+  <si>
+    <t>basic view</t>
+  </si>
+  <si>
+    <t>auto loading of listings when scrolled down</t>
+  </si>
+  <si>
+    <t>list of homestays in chikmagalur</t>
+  </si>
+  <si>
+    <t>list of homestay in chikmagalur</t>
+  </si>
+  <si>
+    <t>book homestay in chikmagalur</t>
+  </si>
+  <si>
+    <t>book homestay in coorg</t>
+  </si>
+  <si>
+    <t>homestay in chikmagalur</t>
+  </si>
+  <si>
+    <t>homestay in coorg</t>
+  </si>
+  <si>
+    <t>http://yourstory.com/2014/03/ultimate-master-list-revenue-models-web-mobile-companies/</t>
+  </si>
+  <si>
+    <t>The ultimate master list of revenue models used by Web and Mobile companies</t>
+  </si>
+  <si>
+    <t>Links</t>
+  </si>
+  <si>
+    <t>Desc</t>
+  </si>
+  <si>
+    <t>holidayiq.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -33,13 +113,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -51,13 +153,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -357,20 +470,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="45.85546875" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -394,12 +563,108 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="50.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86.85546875" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
created folders & roadmap sheet
</commit_message>
<xml_diff>
--- a/notes/bmhs_details.xlsx
+++ b/notes/bmhs_details.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="pages" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -650,7 +650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>

</xml_diff>